<commit_message>
prograsso con grafana e influx
</commit_message>
<xml_diff>
--- a/Default.xlsx
+++ b/Default.xlsx
@@ -5108,7 +5108,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.2"/>
   <cols>
     <col width="9" customWidth="1" style="363" min="1" max="1"/>
     <col width="10.33203125" customWidth="1" style="363" min="2" max="2"/>
@@ -5308,21 +5308,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D7" s="418" t="n">
-        <v>837</v>
-      </c>
-      <c r="E7" s="419" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="419" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G7" s="419" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H7" s="420" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D7" s="418" t="n"/>
+      <c r="E7" s="419" t="n"/>
+      <c r="F7" s="419" t="n"/>
+      <c r="G7" s="419" t="n"/>
+      <c r="H7" s="420" t="n"/>
       <c r="I7" s="364">
         <f>(H7-$E$5)+$H$2</f>
         <v/>
@@ -5377,21 +5367,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D8" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E8" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G8" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H8" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D8" s="421" t="n"/>
+      <c r="E8" s="339" t="n"/>
+      <c r="F8" s="339" t="n"/>
+      <c r="G8" s="339" t="n"/>
+      <c r="H8" s="422" t="n"/>
       <c r="I8" s="365">
         <f>(H8-$E$5)+$H$2</f>
         <v/>
@@ -5446,21 +5426,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D9" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E9" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G9" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H9" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D9" s="421" t="n"/>
+      <c r="E9" s="339" t="n"/>
+      <c r="F9" s="339" t="n"/>
+      <c r="G9" s="339" t="n"/>
+      <c r="H9" s="422" t="n"/>
       <c r="I9" s="365">
         <f>(H9-$E$5)+$H$2</f>
         <v/>
@@ -5515,21 +5485,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D10" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E10" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G10" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H10" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D10" s="421" t="n"/>
+      <c r="E10" s="339" t="n"/>
+      <c r="F10" s="339" t="n"/>
+      <c r="G10" s="339" t="n"/>
+      <c r="H10" s="422" t="n"/>
       <c r="I10" s="365">
         <f>(H10-$E$5)+$H$2</f>
         <v/>
@@ -5584,21 +5544,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D11" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E11" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G11" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H11" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D11" s="421" t="n"/>
+      <c r="E11" s="339" t="n"/>
+      <c r="F11" s="339" t="n"/>
+      <c r="G11" s="339" t="n"/>
+      <c r="H11" s="422" t="n"/>
       <c r="I11" s="365">
         <f>(H11-$E$5)+$H$2</f>
         <v/>
@@ -5653,21 +5603,11 @@
         <f>C_Tar_min</f>
         <v/>
       </c>
-      <c r="D12" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E12" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G12" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H12" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D12" s="421" t="n"/>
+      <c r="E12" s="339" t="n"/>
+      <c r="F12" s="339" t="n"/>
+      <c r="G12" s="339" t="n"/>
+      <c r="H12" s="422" t="n"/>
       <c r="I12" s="365">
         <f>(H12-$E$5)+$H$2</f>
         <v/>
@@ -5722,21 +5662,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D13" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E13" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G13" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H13" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D13" s="423" t="n"/>
+      <c r="E13" s="343" t="n"/>
+      <c r="F13" s="343" t="n"/>
+      <c r="G13" s="343" t="n"/>
+      <c r="H13" s="424" t="n"/>
       <c r="I13" s="364">
         <f>(H13-$E$5)+$H$2</f>
         <v/>
@@ -5791,21 +5721,11 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D14" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E14" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G14" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H14" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D14" s="425" t="n"/>
+      <c r="E14" s="344" t="n"/>
+      <c r="F14" s="344" t="n"/>
+      <c r="G14" s="344" t="n"/>
+      <c r="H14" s="426" t="n"/>
       <c r="I14" s="365">
         <f>(H14-$E$5)+$H$2</f>
         <v/>
@@ -5860,21 +5780,11 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D15" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E15" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G15" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H15" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D15" s="425" t="n"/>
+      <c r="E15" s="344" t="n"/>
+      <c r="F15" s="344" t="n"/>
+      <c r="G15" s="344" t="n"/>
+      <c r="H15" s="426" t="n"/>
       <c r="I15" s="365">
         <f>(H15-$E$5)+$H$2</f>
         <v/>
@@ -5929,21 +5839,11 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D16" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E16" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G16" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H16" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D16" s="425" t="n"/>
+      <c r="E16" s="344" t="n"/>
+      <c r="F16" s="344" t="n"/>
+      <c r="G16" s="344" t="n"/>
+      <c r="H16" s="426" t="n"/>
       <c r="I16" s="365">
         <f>(H16-$E$5)+$H$2</f>
         <v/>
@@ -5998,21 +5898,11 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D17" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E17" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G17" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H17" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D17" s="425" t="n"/>
+      <c r="E17" s="344" t="n"/>
+      <c r="F17" s="344" t="n"/>
+      <c r="G17" s="344" t="n"/>
+      <c r="H17" s="426" t="n"/>
       <c r="I17" s="365">
         <f>(H17-$E$5)+$H$2</f>
         <v/>
@@ -6067,21 +5957,11 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D18" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E18" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G18" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H18" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D18" s="425" t="n"/>
+      <c r="E18" s="344" t="n"/>
+      <c r="F18" s="344" t="n"/>
+      <c r="G18" s="344" t="n"/>
+      <c r="H18" s="426" t="n"/>
       <c r="I18" s="365">
         <f>(H18-$E$5)+$H$2</f>
         <v/>
@@ -6136,21 +6016,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D19" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E19" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="343" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G19" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H19" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D19" s="423" t="n"/>
+      <c r="E19" s="343" t="n"/>
+      <c r="F19" s="343" t="n"/>
+      <c r="G19" s="343" t="n"/>
+      <c r="H19" s="424" t="n"/>
       <c r="I19" s="364">
         <f>(H19-$E$5)+$H$2</f>
         <v/>
@@ -6205,21 +6075,11 @@
         <f>SetPnt_N_1</f>
         <v/>
       </c>
-      <c r="D20" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E20" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G20" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H20" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D20" s="425" t="n"/>
+      <c r="E20" s="344" t="n"/>
+      <c r="F20" s="344" t="n"/>
+      <c r="G20" s="344" t="n"/>
+      <c r="H20" s="426" t="n"/>
       <c r="I20" s="365">
         <f>(H20-$E$5)+$H$2</f>
         <v/>
@@ -6274,21 +6134,11 @@
         <f>SetPnt_N_2</f>
         <v/>
       </c>
-      <c r="D21" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E21" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G21" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H21" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D21" s="425" t="n"/>
+      <c r="E21" s="344" t="n"/>
+      <c r="F21" s="344" t="n"/>
+      <c r="G21" s="344" t="n"/>
+      <c r="H21" s="426" t="n"/>
       <c r="I21" s="365">
         <f>(H21-$E$5)+$H$2</f>
         <v/>
@@ -6343,21 +6193,11 @@
         <f>SetPnt_N_3</f>
         <v/>
       </c>
-      <c r="D22" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E22" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G22" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H22" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D22" s="425" t="n"/>
+      <c r="E22" s="344" t="n"/>
+      <c r="F22" s="344" t="n"/>
+      <c r="G22" s="344" t="n"/>
+      <c r="H22" s="426" t="n"/>
       <c r="I22" s="365">
         <f>(H22-$E$5)+$H$2</f>
         <v/>
@@ -6412,21 +6252,11 @@
         <f>SetPnt_N_4</f>
         <v/>
       </c>
-      <c r="D23" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E23" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G23" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H23" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D23" s="425" t="n"/>
+      <c r="E23" s="344" t="n"/>
+      <c r="F23" s="344" t="n"/>
+      <c r="G23" s="344" t="n"/>
+      <c r="H23" s="426" t="n"/>
       <c r="I23" s="365">
         <f>(H23-$E$5)+$H$2</f>
         <v/>
@@ -6481,21 +6311,11 @@
         <f>SetPnt_N_5</f>
         <v/>
       </c>
-      <c r="D24" s="427" t="n">
-        <v>837</v>
-      </c>
-      <c r="E24" s="348" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="348" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G24" s="348" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H24" s="428" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D24" s="427" t="n"/>
+      <c r="E24" s="348" t="n"/>
+      <c r="F24" s="348" t="n"/>
+      <c r="G24" s="348" t="n"/>
+      <c r="H24" s="428" t="n"/>
       <c r="I24" s="366">
         <f>(H24-$E$5)+$H$2</f>
         <v/>
@@ -6550,21 +6370,11 @@
         <f>SetPnt_N_0</f>
         <v/>
       </c>
-      <c r="D25" s="429" t="n">
-        <v>837</v>
-      </c>
-      <c r="E25" s="430" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="430" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G25" s="430" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H25" s="431" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D25" s="429" t="n"/>
+      <c r="E25" s="430" t="n"/>
+      <c r="F25" s="430" t="n"/>
+      <c r="G25" s="430" t="n"/>
+      <c r="H25" s="431" t="n"/>
       <c r="I25" s="366">
         <f>(H25-$E$5)+$H$2</f>
         <v/>
@@ -6607,20 +6417,14 @@
       </c>
     </row>
     <row r="26" ht="14.4" customFormat="1" customHeight="1" s="327">
-      <c r="D26" s="327" t="n">
-        <v>837</v>
-      </c>
-      <c r="E26" s="327" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G26" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.001</v>
+      <c r="D26" s="327" t="inlineStr">
+        <is>
+          <t>Href</t>
+        </is>
+      </c>
+      <c r="E26" s="327">
+        <f>AVERAGE(E29,E31,E33,E35,E41,E47)</f>
+        <v/>
       </c>
       <c r="O26" s="505" t="n"/>
       <c r="R26" s="505" t="n"/>
@@ -6742,21 +6546,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D29" s="418" t="n">
-        <v>837</v>
-      </c>
-      <c r="E29" s="419" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="419" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G29" s="419" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H29" s="420" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D29" s="418" t="n"/>
+      <c r="E29" s="419" t="n"/>
+      <c r="F29" s="419" t="n"/>
+      <c r="G29" s="419" t="n"/>
+      <c r="H29" s="420" t="n"/>
       <c r="I29" s="364">
         <f>(H29-$E$27)+$H$2</f>
         <v/>
@@ -6811,21 +6605,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D30" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E30" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G30" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H30" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D30" s="421" t="n"/>
+      <c r="E30" s="339" t="n"/>
+      <c r="F30" s="339" t="n"/>
+      <c r="G30" s="339" t="n"/>
+      <c r="H30" s="422" t="n"/>
       <c r="I30" s="365">
         <f>(H30-$E$27)+$H$2</f>
         <v/>
@@ -6880,21 +6664,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D31" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E31" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G31" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H31" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D31" s="421" t="n"/>
+      <c r="E31" s="339" t="n"/>
+      <c r="F31" s="339" t="n"/>
+      <c r="G31" s="339" t="n"/>
+      <c r="H31" s="422" t="n"/>
       <c r="I31" s="365">
         <f>(H31-$E$27)+$H$2</f>
         <v/>
@@ -6949,21 +6723,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D32" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E32" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="339" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G32" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H32" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D32" s="421" t="n"/>
+      <c r="E32" s="339" t="n"/>
+      <c r="F32" s="339" t="n"/>
+      <c r="G32" s="339" t="n"/>
+      <c r="H32" s="422" t="n"/>
       <c r="I32" s="365">
         <f>(H32-$E$27)+$H$2</f>
         <v/>
@@ -7018,21 +6782,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D33" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E33" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G33" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H33" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D33" s="421" t="n"/>
+      <c r="E33" s="339" t="n"/>
+      <c r="F33" s="339" t="n"/>
+      <c r="G33" s="339" t="n"/>
+      <c r="H33" s="422" t="n"/>
       <c r="I33" s="365">
         <f>(H33-$E$27)+$H$2</f>
         <v/>
@@ -7087,21 +6841,11 @@
         <f>C_Tar_max</f>
         <v/>
       </c>
-      <c r="D34" s="421" t="n">
-        <v>837</v>
-      </c>
-      <c r="E34" s="339" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="339" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G34" s="339" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H34" s="422" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D34" s="421" t="n"/>
+      <c r="E34" s="339" t="n"/>
+      <c r="F34" s="339" t="n"/>
+      <c r="G34" s="339" t="n"/>
+      <c r="H34" s="422" t="n"/>
       <c r="I34" s="365">
         <f>(H34-$E$27)+$H$2</f>
         <v/>
@@ -7156,21 +6900,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D35" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E35" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G35" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H35" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D35" s="423" t="n"/>
+      <c r="E35" s="343" t="n"/>
+      <c r="F35" s="343" t="n"/>
+      <c r="G35" s="343" t="n"/>
+      <c r="H35" s="424" t="n"/>
       <c r="I35" s="364">
         <f>(H35-$E$27)+$H$2</f>
         <v/>
@@ -7225,21 +6959,11 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D36" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E36" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G36" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H36" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D36" s="425" t="n"/>
+      <c r="E36" s="344" t="n"/>
+      <c r="F36" s="344" t="n"/>
+      <c r="G36" s="344" t="n"/>
+      <c r="H36" s="426" t="n"/>
       <c r="I36" s="365">
         <f>(H36-$E$27)+$H$2</f>
         <v/>
@@ -7294,21 +7018,11 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D37" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E37" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G37" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H37" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D37" s="425" t="n"/>
+      <c r="E37" s="344" t="n"/>
+      <c r="F37" s="344" t="n"/>
+      <c r="G37" s="344" t="n"/>
+      <c r="H37" s="426" t="n"/>
       <c r="I37" s="365">
         <f>(H37-$E$27)+$H$2</f>
         <v/>
@@ -7363,21 +7077,11 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D38" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E38" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G38" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H38" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D38" s="425" t="n"/>
+      <c r="E38" s="344" t="n"/>
+      <c r="F38" s="344" t="n"/>
+      <c r="G38" s="344" t="n"/>
+      <c r="H38" s="426" t="n"/>
       <c r="I38" s="365">
         <f>(H38-$E$27)+$H$2</f>
         <v/>
@@ -7432,21 +7136,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D39" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E39" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G39" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H39" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D39" s="425" t="n"/>
+      <c r="E39" s="344" t="n"/>
+      <c r="F39" s="344" t="n"/>
+      <c r="G39" s="344" t="n"/>
+      <c r="H39" s="426" t="n"/>
       <c r="I39" s="365">
         <f>(H39-$E$27)+$H$2</f>
         <v/>
@@ -7501,21 +7195,11 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D40" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E40" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G40" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H40" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D40" s="425" t="n"/>
+      <c r="E40" s="344" t="n"/>
+      <c r="F40" s="344" t="n"/>
+      <c r="G40" s="344" t="n"/>
+      <c r="H40" s="426" t="n"/>
       <c r="I40" s="365">
         <f>(H40-$E$27)+$H$2</f>
         <v/>
@@ -7570,21 +7254,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D41" s="423" t="n">
-        <v>837</v>
-      </c>
-      <c r="E41" s="343" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="343" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G41" s="343" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H41" s="424" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D41" s="423" t="n"/>
+      <c r="E41" s="343" t="n"/>
+      <c r="F41" s="343" t="n"/>
+      <c r="G41" s="343" t="n"/>
+      <c r="H41" s="424" t="n"/>
       <c r="I41" s="364">
         <f>(H41-$E$27)+$H$2</f>
         <v/>
@@ -7639,21 +7313,11 @@
         <f>SetPnt_P_1</f>
         <v/>
       </c>
-      <c r="D42" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E42" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G42" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H42" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D42" s="425" t="n"/>
+      <c r="E42" s="344" t="n"/>
+      <c r="F42" s="344" t="n"/>
+      <c r="G42" s="344" t="n"/>
+      <c r="H42" s="426" t="n"/>
       <c r="I42" s="365">
         <f>(H42-$E$27)+$H$2</f>
         <v/>
@@ -7708,21 +7372,11 @@
         <f>SetPnt_P_2</f>
         <v/>
       </c>
-      <c r="D43" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E43" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G43" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H43" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D43" s="425" t="n"/>
+      <c r="E43" s="344" t="n"/>
+      <c r="F43" s="344" t="n"/>
+      <c r="G43" s="344" t="n"/>
+      <c r="H43" s="426" t="n"/>
       <c r="I43" s="365">
         <f>(H43-$E$27)+$H$2</f>
         <v/>
@@ -7777,21 +7431,11 @@
         <f>SetPnt_P_3</f>
         <v/>
       </c>
-      <c r="D44" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E44" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="344" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G44" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H44" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D44" s="425" t="n"/>
+      <c r="E44" s="344" t="n"/>
+      <c r="F44" s="344" t="n"/>
+      <c r="G44" s="344" t="n"/>
+      <c r="H44" s="426" t="n"/>
       <c r="I44" s="365">
         <f>(H44-$E$27)+$H$2</f>
         <v/>
@@ -7846,21 +7490,11 @@
         <f>SetPnt_P_4</f>
         <v/>
       </c>
-      <c r="D45" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E45" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G45" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H45" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D45" s="425" t="n"/>
+      <c r="E45" s="344" t="n"/>
+      <c r="F45" s="344" t="n"/>
+      <c r="G45" s="344" t="n"/>
+      <c r="H45" s="426" t="n"/>
       <c r="I45" s="365">
         <f>(H45-$E$27)+$H$2</f>
         <v/>
@@ -7915,21 +7549,11 @@
         <f>SetPnt_P_5</f>
         <v/>
       </c>
-      <c r="D46" s="425" t="n">
-        <v>837</v>
-      </c>
-      <c r="E46" s="344" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="344" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G46" s="344" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H46" s="426" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D46" s="425" t="n"/>
+      <c r="E46" s="344" t="n"/>
+      <c r="F46" s="344" t="n"/>
+      <c r="G46" s="344" t="n"/>
+      <c r="H46" s="426" t="n"/>
       <c r="I46" s="366">
         <f>(H46-$E$27)+$H$2</f>
         <v/>
@@ -7984,21 +7608,11 @@
         <f>SetPnt_P_0</f>
         <v/>
       </c>
-      <c r="D47" s="429" t="n">
-        <v>837</v>
-      </c>
-      <c r="E47" s="430" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="430" t="n">
-        <v>-157.0411782090434</v>
-      </c>
-      <c r="G47" s="430" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H47" s="431" t="n">
-        <v>0.001</v>
-      </c>
+      <c r="D47" s="429" t="n"/>
+      <c r="E47" s="430" t="n"/>
+      <c r="F47" s="430" t="n"/>
+      <c r="G47" s="430" t="n"/>
+      <c r="H47" s="431" t="n"/>
       <c r="I47" s="366">
         <f>(H47-$E$27)+$H$2</f>
         <v/>
@@ -8040,23 +7654,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" customFormat="1" s="327">
-      <c r="D48" t="n">
-        <v>837</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>-156.5579745837849</v>
-      </c>
-      <c r="G48" t="n">
-        <v>-1.3734</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
+    <row r="48" customFormat="1" s="327"/>
     <row r="49" ht="14.4" customFormat="1" customHeight="1" s="327">
       <c r="I49" s="432" t="inlineStr">
         <is>
@@ -9083,7 +8681,7 @@
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="25.88671875" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
@@ -10674,7 +10272,7 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="15.5546875" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -16897,7 +16495,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col width="14.33203125" customWidth="1" min="1" max="1"/>
     <col width="19.6640625" customWidth="1" min="2" max="2"/>
@@ -23094,7 +22692,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="13.5546875" customWidth="1" min="3" max="3"/>
@@ -24259,7 +23857,7 @@
       <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
     <col width="3.5546875" customWidth="1" min="2" max="2"/>
@@ -25768,8 +25366,8 @@
     <mergeCell ref="F16:M16"/>
     <mergeCell ref="G98:H98"/>
     <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G97:H97"/>
     <mergeCell ref="L102:L103"/>
-    <mergeCell ref="G97:H97"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="I70:J70"/>
     <mergeCell ref="I91:J91"/>

</xml_diff>